<commit_message>
create RentAdjuster class and add functionality to decide if a rent adjustment is wanted
</commit_message>
<xml_diff>
--- a/src/main/resources/sample/Indexmieten_Übersicht.xlsx
+++ b/src/main/resources/sample/Indexmieten_Übersicht.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\IdeaProjects\rent-index\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\IdeaProjects\rent-index\src\main\resources\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE550D8-9659-416F-8F66-2D99503EBAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D9E11A-8ABA-46D5-B824-8B1E96A317A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Mieter</t>
   </si>
@@ -97,27 +97,18 @@
     <t>HR</t>
   </si>
   <si>
-    <t>unmod.</t>
-  </si>
-  <si>
     <t>Gasöfen</t>
   </si>
   <si>
     <t>April</t>
   </si>
   <si>
-    <t>modern.</t>
-  </si>
-  <si>
     <t>Therme</t>
   </si>
   <si>
     <t>Dezember</t>
   </si>
   <si>
-    <t>teilmod.</t>
-  </si>
-  <si>
     <t>2. re</t>
   </si>
   <si>
@@ -182,6 +173,18 @@
   </si>
   <si>
     <t>Beheizung</t>
+  </si>
+  <si>
+    <t>unmod</t>
+  </si>
+  <si>
+    <t>mod</t>
+  </si>
+  <si>
+    <t>teilmod</t>
+  </si>
+  <si>
+    <t>MAX</t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -283,13 +286,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -595,7 +591,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:X23"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -623,7 +619,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -635,7 +631,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>7</v>
@@ -688,10 +684,10 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2">
         <v>44</v>
@@ -704,16 +700,16 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
         <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
       </c>
       <c r="K2">
         <v>2023</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M2">
         <v>720</v>
@@ -728,32 +724,32 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2">
         <v>64</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K3">
         <v>2022</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M3">
         <v>945</v>
@@ -768,38 +764,38 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="5">
         <v>104</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
       </c>
       <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
         <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
       </c>
       <c r="K4">
         <v>2023</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M4">
         <v>1345</v>
@@ -814,35 +810,35 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" s="5">
         <v>74</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K5">
         <v>2022</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M5">
         <v>1122</v>
@@ -860,32 +856,35 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D6" s="5">
         <v>34</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
       </c>
       <c r="K6">
         <v>2023</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M6">
         <v>544</v>
@@ -937,209 +936,47 @@
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D29" s="5"/>
       <c r="J29" s="8"/>
     </row>

</xml_diff>

<commit_message>
more bug fixes, should work now and produces an overview
</commit_message>
<xml_diff>
--- a/src/main/resources/sample/Indexmieten_Übersicht.xlsx
+++ b/src/main/resources/sample/Indexmieten_Übersicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\IdeaProjects\rent-index\src\main\resources\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D9E11A-8ABA-46D5-B824-8B1E96A317A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499782E1-EE25-4E3E-8074-B8E1A4F815C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Mieter</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>MAX</t>
+  </si>
+  <si>
+    <t>Grund</t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -602,10 +605,10 @@
     <col min="7" max="7" width="6.7265625" customWidth="1"/>
     <col min="8" max="9" width="8.7265625" customWidth="1"/>
     <col min="10" max="10" width="10.453125" customWidth="1"/>
-    <col min="26" max="26" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,19 +673,22 @@
         <v>18</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -722,7 +728,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -762,7 +768,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -808,7 +814,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -854,7 +860,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -900,39 +906,39 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D7" s="2"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
     </row>

</xml_diff>

<commit_message>
add letter template and BuildingDataLoader. Also rename some methods
</commit_message>
<xml_diff>
--- a/src/main/resources/sample/Indexmieten_Übersicht.xlsx
+++ b/src/main/resources/sample/Indexmieten_Übersicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\IdeaProjects\rent-index\src\main\resources\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499782E1-EE25-4E3E-8074-B8E1A4F815C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958C8A22-DE1E-4BC9-AFD5-801BC323BD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Mieter</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>teilmod</t>
-  </si>
-  <si>
-    <t>MAX</t>
   </si>
   <si>
     <t>Grund</t>
@@ -594,7 +591,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,7 +670,7 @@
         <v>18</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>19</v>
@@ -882,9 +879,6 @@
       </c>
       <c r="I6" t="s">
         <v>34</v>
-      </c>
-      <c r="J6" t="s">
-        <v>54</v>
       </c>
       <c r="K6">
         <v>2023</v>

</xml_diff>

<commit_message>
add LetterWriter and other small changes
</commit_message>
<xml_diff>
--- a/src/main/resources/sample/Indexmieten_Übersicht.xlsx
+++ b/src/main/resources/sample/Indexmieten_Übersicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\IdeaProjects\rent-index\src\main\resources\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958C8A22-DE1E-4BC9-AFD5-801BC323BD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A7C99E-73DF-47A1-92CC-C93482AAC534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1380" windowWidth="19190" windowHeight="10190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -266,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -286,6 +286,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -590,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2:X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -724,6 +725,8 @@
       <c r="O2">
         <v>60</v>
       </c>
+      <c r="U2" s="9"/>
+      <c r="X2" s="9"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -764,6 +767,8 @@
       <c r="O3">
         <v>90</v>
       </c>
+      <c r="U3" s="9"/>
+      <c r="X3" s="9"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -810,6 +815,8 @@
       <c r="O4">
         <v>145</v>
       </c>
+      <c r="U4" s="9"/>
+      <c r="X4" s="9"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -856,6 +863,8 @@
       <c r="P5">
         <v>100</v>
       </c>
+      <c r="U5" s="9"/>
+      <c r="X5" s="9"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -899,14 +908,19 @@
       <c r="P6">
         <v>80</v>
       </c>
+      <c r="U6" s="9"/>
+      <c r="X6" s="9"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D7" s="2"/>
       <c r="E7" s="6"/>
+      <c r="U7" s="9"/>
+      <c r="X7" s="9"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
+      <c r="X8" s="9"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D9" s="5"/>

</xml_diff>